<commit_message>
Fix bug for IR and FX classes and reorganize code structure
</commit_message>
<xml_diff>
--- a/simm_config.xlsx
+++ b/simm_config.xlsx
@@ -4,23 +4,25 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="8250" activeTab="6"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="8250" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
-    <sheet name="IR_weights" sheetId="1" r:id="rId1"/>
-    <sheet name="IR_correlation" sheetId="2" r:id="rId2"/>
-    <sheet name="IR_CR_THR" sheetId="3" r:id="rId3"/>
-    <sheet name="CreditQ_weights" sheetId="4" r:id="rId4"/>
-    <sheet name="CreditQ_correlation" sheetId="5" r:id="rId5"/>
-    <sheet name="CreditQ_CR_THR" sheetId="6" r:id="rId6"/>
-    <sheet name="FX_CR_THR" sheetId="8" r:id="rId7"/>
+    <sheet name="run_cases" sheetId="10" r:id="rId1"/>
+    <sheet name="simm_input" sheetId="9" r:id="rId2"/>
+    <sheet name="IR_weights" sheetId="1" r:id="rId3"/>
+    <sheet name="IR_correlation" sheetId="2" r:id="rId4"/>
+    <sheet name="IR_CR_THR" sheetId="3" r:id="rId5"/>
+    <sheet name="CreditQ_weights" sheetId="4" r:id="rId6"/>
+    <sheet name="CreditQ_correlation" sheetId="5" r:id="rId7"/>
+    <sheet name="CreditQ_CR_THR" sheetId="6" r:id="rId8"/>
+    <sheet name="FX_CR_THR" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="206">
   <si>
     <t>curr</t>
   </si>
@@ -76,18 +78,6 @@
     <t>Delta</t>
   </si>
   <si>
-    <t>High_Vol</t>
-  </si>
-  <si>
-    <t>Reg_Vol_Well_Traded</t>
-  </si>
-  <si>
-    <t>Reg_Vol_Less_Well_Traded</t>
-  </si>
-  <si>
-    <t>Low_Vol</t>
-  </si>
-  <si>
     <t>Vega</t>
   </si>
   <si>
@@ -131,6 +121,525 @@
   </si>
   <si>
     <t>C3</t>
+  </si>
+  <si>
+    <t>High volatility</t>
+  </si>
+  <si>
+    <t>Low volatility</t>
+  </si>
+  <si>
+    <t>Regular volatility, less well-traded</t>
+  </si>
+  <si>
+    <t>Regular volatility, well-traded</t>
+  </si>
+  <si>
+    <t>ProductClass</t>
+  </si>
+  <si>
+    <t>SensitivityID</t>
+  </si>
+  <si>
+    <t>RiskType</t>
+  </si>
+  <si>
+    <t>Qualifier</t>
+  </si>
+  <si>
+    <t>Bucket</t>
+  </si>
+  <si>
+    <t>Label1</t>
+  </si>
+  <si>
+    <t>Label2</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>AmoutCurrency</t>
+  </si>
+  <si>
+    <t>AmountUSD</t>
+  </si>
+  <si>
+    <t>RatesFX</t>
+  </si>
+  <si>
+    <t>S_IR_1</t>
+  </si>
+  <si>
+    <t>Risk_IRCurve</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>10y</t>
+  </si>
+  <si>
+    <t>Libor3m</t>
+  </si>
+  <si>
+    <t>S_IR_2</t>
+  </si>
+  <si>
+    <t>5y</t>
+  </si>
+  <si>
+    <t>Libor1m</t>
+  </si>
+  <si>
+    <t>S_IR_3</t>
+  </si>
+  <si>
+    <t>2y</t>
+  </si>
+  <si>
+    <t>OIS</t>
+  </si>
+  <si>
+    <t>S_IR_4</t>
+  </si>
+  <si>
+    <t>Risk_Inflation</t>
+  </si>
+  <si>
+    <t>S_IR_5</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>S_IR_6</t>
+  </si>
+  <si>
+    <t>20y</t>
+  </si>
+  <si>
+    <t>S_IR_7</t>
+  </si>
+  <si>
+    <t>GBP</t>
+  </si>
+  <si>
+    <t>S_IR_8</t>
+  </si>
+  <si>
+    <t>JPY</t>
+  </si>
+  <si>
+    <t>S_IR_9</t>
+  </si>
+  <si>
+    <t>S_IR_10</t>
+  </si>
+  <si>
+    <t>AUD</t>
+  </si>
+  <si>
+    <t>S_IR_11</t>
+  </si>
+  <si>
+    <t>INR</t>
+  </si>
+  <si>
+    <t>S_IR_12</t>
+  </si>
+  <si>
+    <t>CNY</t>
+  </si>
+  <si>
+    <t>S_IR_13</t>
+  </si>
+  <si>
+    <t>S_IR_14</t>
+  </si>
+  <si>
+    <t>S_IR_15</t>
+  </si>
+  <si>
+    <t>Equity</t>
+  </si>
+  <si>
+    <t>S_CRQ_1</t>
+  </si>
+  <si>
+    <t>Risk_CreditQ</t>
+  </si>
+  <si>
+    <t>ISIN:BE0934259525</t>
+  </si>
+  <si>
+    <t>1y</t>
+  </si>
+  <si>
+    <t>S_CRQ_2</t>
+  </si>
+  <si>
+    <t>sec</t>
+  </si>
+  <si>
+    <t>S_FX_1a</t>
+  </si>
+  <si>
+    <t>Risk_FX</t>
+  </si>
+  <si>
+    <t>S_FX_1b</t>
+  </si>
+  <si>
+    <t>S_FX_2a</t>
+  </si>
+  <si>
+    <t>S_FX_2b</t>
+  </si>
+  <si>
+    <t>S_FX_3a</t>
+  </si>
+  <si>
+    <t>S_FX_3b</t>
+  </si>
+  <si>
+    <t>S_FX_4a</t>
+  </si>
+  <si>
+    <t>S_FX_4b</t>
+  </si>
+  <si>
+    <t>RUB</t>
+  </si>
+  <si>
+    <t>S_EQ_1</t>
+  </si>
+  <si>
+    <t>Risk_Equity</t>
+  </si>
+  <si>
+    <t>ISIN:AT0000730007</t>
+  </si>
+  <si>
+    <t>S_EQ_2</t>
+  </si>
+  <si>
+    <t>ISIN:AT0000937503</t>
+  </si>
+  <si>
+    <t>Credit</t>
+  </si>
+  <si>
+    <t>S_EQ_12</t>
+  </si>
+  <si>
+    <t>ISIN:UNKNOWN1</t>
+  </si>
+  <si>
+    <t>Commodity</t>
+  </si>
+  <si>
+    <t>S_CM_1</t>
+  </si>
+  <si>
+    <t>Risk_Commodity</t>
+  </si>
+  <si>
+    <t>NA Natural Gas Gulf Coast</t>
+  </si>
+  <si>
+    <t>S_CM_2</t>
+  </si>
+  <si>
+    <t>Crude Oil Americas</t>
+  </si>
+  <si>
+    <t>S_IRV_1</t>
+  </si>
+  <si>
+    <t>Risk_IRVol</t>
+  </si>
+  <si>
+    <t>S_IRV_2</t>
+  </si>
+  <si>
+    <t>S_IRV_3</t>
+  </si>
+  <si>
+    <t>S_IRV_4</t>
+  </si>
+  <si>
+    <t>S_IRV_5</t>
+  </si>
+  <si>
+    <t>S_IRV_6</t>
+  </si>
+  <si>
+    <t>S_IRV_7</t>
+  </si>
+  <si>
+    <t>S_IRV_8</t>
+  </si>
+  <si>
+    <t>S_FXV1</t>
+  </si>
+  <si>
+    <t>Risk_FXVol</t>
+  </si>
+  <si>
+    <t>USDGBP</t>
+  </si>
+  <si>
+    <t>S_FXV2</t>
+  </si>
+  <si>
+    <t>GBPUSD</t>
+  </si>
+  <si>
+    <t>S_FXV3</t>
+  </si>
+  <si>
+    <t>USDAUD</t>
+  </si>
+  <si>
+    <t>S_FXV4</t>
+  </si>
+  <si>
+    <t>EURUSD</t>
+  </si>
+  <si>
+    <t>S_FXV5</t>
+  </si>
+  <si>
+    <t>AUDJPY</t>
+  </si>
+  <si>
+    <t>S_FXV6</t>
+  </si>
+  <si>
+    <t>CNYSGD</t>
+  </si>
+  <si>
+    <t>CombinationID</t>
+  </si>
+  <si>
+    <t>S_IR_1,S_IR_2</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>C13</t>
+  </si>
+  <si>
+    <t>C14</t>
+  </si>
+  <si>
+    <t>C15</t>
+  </si>
+  <si>
+    <t>C16</t>
+  </si>
+  <si>
+    <t>S_FX_1a,S_FX_1b</t>
+  </si>
+  <si>
+    <t>C17</t>
+  </si>
+  <si>
+    <t>C18</t>
+  </si>
+  <si>
+    <t>C19</t>
+  </si>
+  <si>
+    <t>C20</t>
+  </si>
+  <si>
+    <t>C21</t>
+  </si>
+  <si>
+    <t>C22</t>
+  </si>
+  <si>
+    <t>S_FX_2a,S_FX_2b</t>
+  </si>
+  <si>
+    <t>S_FX_3a,S_FX_3b</t>
+  </si>
+  <si>
+    <t>S_FX_4a,S_FX_4b</t>
+  </si>
+  <si>
+    <t>S_IR_1,S_IR_3</t>
+  </si>
+  <si>
+    <t>S_IR_2,S_IR_3</t>
+  </si>
+  <si>
+    <t>C23</t>
+  </si>
+  <si>
+    <t>C24</t>
+  </si>
+  <si>
+    <t>C25</t>
+  </si>
+  <si>
+    <t>C26</t>
+  </si>
+  <si>
+    <t>C27</t>
+  </si>
+  <si>
+    <t>C28</t>
+  </si>
+  <si>
+    <t>C29</t>
+  </si>
+  <si>
+    <t>C30</t>
+  </si>
+  <si>
+    <t>C31</t>
+  </si>
+  <si>
+    <t>Include</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>S_IR_8,S_IR_9</t>
+  </si>
+  <si>
+    <t>S_IR_2,S_IR_4</t>
+  </si>
+  <si>
+    <t>S_IR_10,S_IR_11</t>
+  </si>
+  <si>
+    <t>S_IR_5,S_IR_7</t>
+  </si>
+  <si>
+    <t>S_IR_1,S_IR_5,S_IR_6</t>
+  </si>
+  <si>
+    <t>S_IR_3,S_IR_13,S_IR_14</t>
+  </si>
+  <si>
+    <t>S_IR_2,S_IR_3,S_IR_12,S_IR_15</t>
+  </si>
+  <si>
+    <t>S_FX_1a,S_FX_1b,S_FX_3a,S_FX_3b</t>
+  </si>
+  <si>
+    <t>C32</t>
+  </si>
+  <si>
+    <t>C33</t>
+  </si>
+  <si>
+    <t>C34</t>
+  </si>
+  <si>
+    <t>C35</t>
+  </si>
+  <si>
+    <t>C36</t>
+  </si>
+  <si>
+    <t>C37</t>
+  </si>
+  <si>
+    <t>C38</t>
+  </si>
+  <si>
+    <t>C39</t>
+  </si>
+  <si>
+    <t>C40</t>
+  </si>
+  <si>
+    <t>C41</t>
+  </si>
+  <si>
+    <t>C42</t>
+  </si>
+  <si>
+    <t>C43</t>
+  </si>
+  <si>
+    <t>C44</t>
+  </si>
+  <si>
+    <t>C45</t>
+  </si>
+  <si>
+    <t>C46</t>
+  </si>
+  <si>
+    <t>C47</t>
+  </si>
+  <si>
+    <t>C48</t>
+  </si>
+  <si>
+    <t>C49</t>
+  </si>
+  <si>
+    <t>C50</t>
+  </si>
+  <si>
+    <t>C51</t>
+  </si>
+  <si>
+    <t>C52</t>
+  </si>
+  <si>
+    <t>C53</t>
+  </si>
+  <si>
+    <t>C54</t>
+  </si>
+  <si>
+    <t>S_FX_1a,S_FX_1b,S_FX_2a,S_FX_2b</t>
+  </si>
+  <si>
+    <t>S_FX_2a,S_FX_2b,S_FX_4a,S_FX_4b</t>
+  </si>
+  <si>
+    <t>S_IR_1,S_FX_1a,S_FX_1b</t>
+  </si>
+  <si>
+    <t>S_IR_1,S_FX_4a,S_FX_4b</t>
+  </si>
+  <si>
+    <t>S_IR_3,S_IR_13,S_IR_15</t>
   </si>
 </sst>
 </file>
@@ -615,12 +1124,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -963,13 +1475,1826 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C55"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B17" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B22" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B23" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B24" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J52"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="4">
+        <v>10000000</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" s="4">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="4">
+        <v>-15000000</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" s="4">
+        <v>-15000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" s="4">
+        <v>5000000</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J4" s="4">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4">
+        <v>-10000000</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" s="4">
+        <v>-10000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" s="4">
+        <v>-20000000</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" s="4">
+        <v>-20000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" s="4">
+        <v>5000000</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J7" s="4">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4">
+        <v>10000000</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J8" s="4">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" s="4">
+        <v>2</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" s="4">
+        <v>-20000000</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J9" s="4">
+        <v>-20000000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="4">
+        <v>2</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10" s="4">
+        <v>10000000</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J10" s="4">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="4">
+        <v>1</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" s="4">
+        <v>5000000</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J11" s="4">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="4">
+        <v>3</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H12" s="4">
+        <v>5000000</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J12" s="4">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4">
+        <v>-10000000</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J13" s="4">
+        <v>-10000000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="4">
+        <v>3</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H14" s="4">
+        <v>10000000</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J14" s="4">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" s="4">
+        <v>3</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H15" s="4">
+        <v>-20000000</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J15" s="4">
+        <v>-20000000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="4">
+        <v>3</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H16" s="4">
+        <v>5000000</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J16" s="4">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E19" s="4">
+        <v>2</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4">
+        <v>10000</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J19" s="4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="4">
+        <v>2</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H20" s="4">
+        <v>-10000</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J20" s="4">
+        <v>-10000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4">
+        <v>1000000000</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J22" s="4">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4">
+        <v>-1000000000</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J23" s="4">
+        <v>-1000000000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4">
+        <v>-1500000000</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J24" s="4">
+        <v>-1500000000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4">
+        <v>1500000000</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J25" s="4">
+        <v>1500000000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4">
+        <v>6000000000</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J26" s="4">
+        <v>6000000000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4">
+        <v>-6000000000</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J27" s="4">
+        <v>-6000000000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4">
+        <v>-2300000000</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J28" s="4">
+        <v>-2300000000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4">
+        <v>2300000000</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J29" s="4">
+        <v>2300000000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E31" s="4">
+        <v>6</v>
+      </c>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4">
+        <v>20000</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J31" s="4">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E32" s="4">
+        <v>7</v>
+      </c>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4">
+        <v>-40000</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J32" s="4">
+        <v>-40000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4">
+        <v>20000</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J33" s="4">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E35" s="4">
+        <v>6</v>
+      </c>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4">
+        <v>20000</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J35" s="4">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E36" s="4">
+        <v>2</v>
+      </c>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4">
+        <v>-40000</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J36" s="4">
+        <v>-40000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4">
+        <v>500000000</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J38" s="4">
+        <v>500000000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4">
+        <v>-500000000</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J39" s="4">
+        <v>-500000000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4">
+        <v>300000000</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J40" s="4">
+        <v>300000000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4">
+        <v>200000000</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J41" s="4">
+        <v>200000000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4">
+        <v>-100000000</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J42" s="4">
+        <v>-100000000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4">
+        <v>20000000</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J43" s="4">
+        <v>20000000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4">
+        <v>150000000</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J44" s="4">
+        <v>150000000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4">
+        <v>-100000000</v>
+      </c>
+      <c r="I45" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J45" s="4">
+        <v>-100000000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4">
+        <v>10000000</v>
+      </c>
+      <c r="I47" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J47" s="4">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4">
+        <v>-50000000</v>
+      </c>
+      <c r="I48" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J48" s="4">
+        <v>-50000000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4">
+        <v>4500000</v>
+      </c>
+      <c r="I49" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J49" s="4">
+        <v>4500000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4">
+        <v>20000000</v>
+      </c>
+      <c r="I50" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J50" s="4">
+        <v>20000000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4">
+        <v>-10000000</v>
+      </c>
+      <c r="I51" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J51" s="4">
+        <v>-10000000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4">
+        <v>90000000</v>
+      </c>
+      <c r="I52" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J52" s="4">
+        <v>90000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,40 +3345,40 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>0.77</v>
+        <v>77</v>
       </c>
       <c r="C2" s="1">
-        <v>0.77</v>
+        <v>77</v>
       </c>
       <c r="D2" s="1">
-        <v>0.77</v>
+        <v>77</v>
       </c>
       <c r="E2" s="1">
-        <v>0.64</v>
+        <v>64</v>
       </c>
       <c r="F2" s="1">
-        <v>0.57999999999999996</v>
+        <v>57.999999999999993</v>
       </c>
       <c r="G2" s="1">
-        <v>0.49</v>
+        <v>49</v>
       </c>
       <c r="H2" s="1">
-        <v>0.47</v>
+        <v>47</v>
       </c>
       <c r="I2" s="1">
-        <v>0.47</v>
+        <v>47</v>
       </c>
       <c r="J2" s="1">
-        <v>0.45</v>
+        <v>45</v>
       </c>
       <c r="K2" s="1">
-        <v>0.45</v>
+        <v>45</v>
       </c>
       <c r="L2" s="1">
-        <v>0.48</v>
+        <v>48</v>
       </c>
       <c r="M2" s="1">
-        <v>0.56000000000000005</v>
+        <v>56.000000000000007</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1061,40 +3386,40 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>0.1</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1">
-        <v>0.1</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1">
-        <v>0.1</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1">
-        <v>0.1</v>
+        <v>10</v>
       </c>
       <c r="F3" s="1">
-        <v>0.13</v>
+        <v>13</v>
       </c>
       <c r="G3" s="1">
-        <v>0.16</v>
+        <v>16</v>
       </c>
       <c r="H3" s="1">
-        <v>0.18</v>
+        <v>18</v>
       </c>
       <c r="I3" s="1">
-        <v>0.2</v>
+        <v>20</v>
       </c>
       <c r="J3" s="1">
-        <v>0.25</v>
+        <v>25</v>
       </c>
       <c r="K3" s="1">
-        <v>0.22</v>
+        <v>22</v>
       </c>
       <c r="L3" s="1">
-        <v>0.22</v>
+        <v>22</v>
       </c>
       <c r="M3" s="1">
-        <v>0.23</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1102,48 +3427,89 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>0.89</v>
+        <v>89</v>
       </c>
       <c r="C4" s="1">
-        <v>0.89</v>
+        <v>89</v>
       </c>
       <c r="D4" s="1">
-        <v>0.89</v>
+        <v>89</v>
       </c>
       <c r="E4" s="1">
-        <v>0.94</v>
+        <v>94</v>
       </c>
       <c r="F4" s="1">
-        <v>1.04</v>
+        <v>104</v>
       </c>
       <c r="G4" s="1">
-        <v>0.99</v>
+        <v>99</v>
       </c>
       <c r="H4" s="1">
-        <v>0.96</v>
+        <v>96</v>
       </c>
       <c r="I4" s="1">
-        <v>0.99</v>
+        <v>99</v>
       </c>
       <c r="J4" s="1">
-        <v>0.87</v>
+        <v>87</v>
       </c>
       <c r="K4" s="1">
-        <v>0.97</v>
+        <v>97</v>
       </c>
       <c r="L4" s="1">
-        <v>0.97</v>
+        <v>97</v>
       </c>
       <c r="M4" s="1">
-        <v>0.98</v>
-      </c>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -1655,7 +4021,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -1663,7 +4029,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C9"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1685,7 +4051,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B2">
         <v>7400000</v>
@@ -1696,7 +4062,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B3">
         <v>250000000</v>
@@ -1707,7 +4073,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B4">
         <v>25000000</v>
@@ -1718,7 +4084,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B5">
         <v>17000000</v>
@@ -1728,47 +4094,47 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>18</v>
+      <c r="A6" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="B6">
         <v>120000000</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B7">
         <v>3070000000</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>20</v>
+      <c r="A8" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="B8">
         <v>160000000</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>21</v>
+      <c r="A9" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="B9">
         <v>960000000</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1777,7 +4143,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -1796,10 +4162,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1900,7 +4266,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B14" s="3">
         <v>6.38</v>
@@ -1911,7 +4277,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -2423,14 +4789,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
@@ -2453,7 +4819,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B2" s="4">
         <v>1000000</v>
@@ -2464,7 +4830,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B3" s="4">
         <v>360000</v>
@@ -2475,7 +4841,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B4" s="4">
         <v>360000</v>
@@ -2486,13 +4852,13 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B5" s="4">
         <v>210000000</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -2500,15 +4866,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2530,7 +4896,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B2" s="4">
         <v>5200000000</v>
@@ -2541,7 +4907,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B3" s="4">
         <v>1300000000</v>
@@ -2552,7 +4918,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B4" s="4">
         <v>260000000</v>
@@ -2563,49 +4929,50 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B5">
         <v>5500000000</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B6">
         <v>3020000000</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B7">
         <v>520000000</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B8">
         <v>87000000</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update readme for run instructions
</commit_message>
<xml_diff>
--- a/simm_config.xlsx
+++ b/simm_config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="8250" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="8250"/>
   </bookViews>
   <sheets>
     <sheet name="run_cases" sheetId="10" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="466">
   <si>
     <t>curr</t>
   </si>
@@ -640,6 +640,786 @@
   </si>
   <si>
     <t>S_IR_3,S_IR_13,S_IR_15</t>
+  </si>
+  <si>
+    <t>C55</t>
+  </si>
+  <si>
+    <t>C56</t>
+  </si>
+  <si>
+    <t>C57</t>
+  </si>
+  <si>
+    <t>C58</t>
+  </si>
+  <si>
+    <t>C59</t>
+  </si>
+  <si>
+    <t>C60</t>
+  </si>
+  <si>
+    <t>C61</t>
+  </si>
+  <si>
+    <t>C62</t>
+  </si>
+  <si>
+    <t>C63</t>
+  </si>
+  <si>
+    <t>C64</t>
+  </si>
+  <si>
+    <t>C65</t>
+  </si>
+  <si>
+    <t>C66</t>
+  </si>
+  <si>
+    <t>C67</t>
+  </si>
+  <si>
+    <t>C68</t>
+  </si>
+  <si>
+    <t>C69</t>
+  </si>
+  <si>
+    <t>C70</t>
+  </si>
+  <si>
+    <t>C71</t>
+  </si>
+  <si>
+    <t>C72</t>
+  </si>
+  <si>
+    <t>C73</t>
+  </si>
+  <si>
+    <t>C74</t>
+  </si>
+  <si>
+    <t>C75</t>
+  </si>
+  <si>
+    <t>C76</t>
+  </si>
+  <si>
+    <t>C77</t>
+  </si>
+  <si>
+    <t>C78</t>
+  </si>
+  <si>
+    <t>C79</t>
+  </si>
+  <si>
+    <t>C80</t>
+  </si>
+  <si>
+    <t>C81</t>
+  </si>
+  <si>
+    <t>C82</t>
+  </si>
+  <si>
+    <t>C83</t>
+  </si>
+  <si>
+    <t>C84</t>
+  </si>
+  <si>
+    <t>C85</t>
+  </si>
+  <si>
+    <t>C86</t>
+  </si>
+  <si>
+    <t>C87</t>
+  </si>
+  <si>
+    <t>C88</t>
+  </si>
+  <si>
+    <t>C89</t>
+  </si>
+  <si>
+    <t>C90</t>
+  </si>
+  <si>
+    <t>C91</t>
+  </si>
+  <si>
+    <t>C92</t>
+  </si>
+  <si>
+    <t>C93</t>
+  </si>
+  <si>
+    <t>C94</t>
+  </si>
+  <si>
+    <t>C95</t>
+  </si>
+  <si>
+    <t>C96</t>
+  </si>
+  <si>
+    <t>C97</t>
+  </si>
+  <si>
+    <t>C98</t>
+  </si>
+  <si>
+    <t>C99</t>
+  </si>
+  <si>
+    <t>C100</t>
+  </si>
+  <si>
+    <t>C101</t>
+  </si>
+  <si>
+    <t>C102</t>
+  </si>
+  <si>
+    <t>C103</t>
+  </si>
+  <si>
+    <t>C104</t>
+  </si>
+  <si>
+    <t>C105</t>
+  </si>
+  <si>
+    <t>C106</t>
+  </si>
+  <si>
+    <t>C107</t>
+  </si>
+  <si>
+    <t>C108</t>
+  </si>
+  <si>
+    <t>C109</t>
+  </si>
+  <si>
+    <t>C110</t>
+  </si>
+  <si>
+    <t>C111</t>
+  </si>
+  <si>
+    <t>C112</t>
+  </si>
+  <si>
+    <t>C113</t>
+  </si>
+  <si>
+    <t>C114</t>
+  </si>
+  <si>
+    <t>C115</t>
+  </si>
+  <si>
+    <t>C116</t>
+  </si>
+  <si>
+    <t>C117</t>
+  </si>
+  <si>
+    <t>C118</t>
+  </si>
+  <si>
+    <t>C119</t>
+  </si>
+  <si>
+    <t>C120</t>
+  </si>
+  <si>
+    <t>C121</t>
+  </si>
+  <si>
+    <t>C122</t>
+  </si>
+  <si>
+    <t>C123</t>
+  </si>
+  <si>
+    <t>C124</t>
+  </si>
+  <si>
+    <t>C125</t>
+  </si>
+  <si>
+    <t>C126</t>
+  </si>
+  <si>
+    <t>C127</t>
+  </si>
+  <si>
+    <t>C128</t>
+  </si>
+  <si>
+    <t>C129</t>
+  </si>
+  <si>
+    <t>C130</t>
+  </si>
+  <si>
+    <t>C131</t>
+  </si>
+  <si>
+    <t>C132</t>
+  </si>
+  <si>
+    <t>C133</t>
+  </si>
+  <si>
+    <t>C134</t>
+  </si>
+  <si>
+    <t>C135</t>
+  </si>
+  <si>
+    <t>C136</t>
+  </si>
+  <si>
+    <t>C137</t>
+  </si>
+  <si>
+    <t>C138</t>
+  </si>
+  <si>
+    <t>C139</t>
+  </si>
+  <si>
+    <t>C140</t>
+  </si>
+  <si>
+    <t>C141</t>
+  </si>
+  <si>
+    <t>C142</t>
+  </si>
+  <si>
+    <t>C143</t>
+  </si>
+  <si>
+    <t>C144</t>
+  </si>
+  <si>
+    <t>C145</t>
+  </si>
+  <si>
+    <t>C146</t>
+  </si>
+  <si>
+    <t>C147</t>
+  </si>
+  <si>
+    <t>C148</t>
+  </si>
+  <si>
+    <t>C149</t>
+  </si>
+  <si>
+    <t>C150</t>
+  </si>
+  <si>
+    <t>C151</t>
+  </si>
+  <si>
+    <t>C152</t>
+  </si>
+  <si>
+    <t>C153</t>
+  </si>
+  <si>
+    <t>C154</t>
+  </si>
+  <si>
+    <t>C155</t>
+  </si>
+  <si>
+    <t>C156</t>
+  </si>
+  <si>
+    <t>C157</t>
+  </si>
+  <si>
+    <t>C158</t>
+  </si>
+  <si>
+    <t>C159</t>
+  </si>
+  <si>
+    <t>C160</t>
+  </si>
+  <si>
+    <t>C161</t>
+  </si>
+  <si>
+    <t>C162</t>
+  </si>
+  <si>
+    <t>C163</t>
+  </si>
+  <si>
+    <t>C164</t>
+  </si>
+  <si>
+    <t>C165</t>
+  </si>
+  <si>
+    <t>C166</t>
+  </si>
+  <si>
+    <t>C167</t>
+  </si>
+  <si>
+    <t>C168</t>
+  </si>
+  <si>
+    <t>C169</t>
+  </si>
+  <si>
+    <t>C170</t>
+  </si>
+  <si>
+    <t>C171</t>
+  </si>
+  <si>
+    <t>C172</t>
+  </si>
+  <si>
+    <t>C173</t>
+  </si>
+  <si>
+    <t>C174</t>
+  </si>
+  <si>
+    <t>C175</t>
+  </si>
+  <si>
+    <t>C176</t>
+  </si>
+  <si>
+    <t>C177</t>
+  </si>
+  <si>
+    <t>C178</t>
+  </si>
+  <si>
+    <t>C179</t>
+  </si>
+  <si>
+    <t>C180</t>
+  </si>
+  <si>
+    <t>C181</t>
+  </si>
+  <si>
+    <t>C182</t>
+  </si>
+  <si>
+    <t>C183</t>
+  </si>
+  <si>
+    <t>C184</t>
+  </si>
+  <si>
+    <t>C185</t>
+  </si>
+  <si>
+    <t>C186</t>
+  </si>
+  <si>
+    <t>C187</t>
+  </si>
+  <si>
+    <t>C188</t>
+  </si>
+  <si>
+    <t>C189</t>
+  </si>
+  <si>
+    <t>C190</t>
+  </si>
+  <si>
+    <t>C191</t>
+  </si>
+  <si>
+    <t>C192</t>
+  </si>
+  <si>
+    <t>C193</t>
+  </si>
+  <si>
+    <t>C194</t>
+  </si>
+  <si>
+    <t>C195</t>
+  </si>
+  <si>
+    <t>C196</t>
+  </si>
+  <si>
+    <t>C197</t>
+  </si>
+  <si>
+    <t>C198</t>
+  </si>
+  <si>
+    <t>C199</t>
+  </si>
+  <si>
+    <t>C200</t>
+  </si>
+  <si>
+    <t>C201</t>
+  </si>
+  <si>
+    <t>C202</t>
+  </si>
+  <si>
+    <t>C203</t>
+  </si>
+  <si>
+    <t>C204</t>
+  </si>
+  <si>
+    <t>C205</t>
+  </si>
+  <si>
+    <t>C206</t>
+  </si>
+  <si>
+    <t>C207</t>
+  </si>
+  <si>
+    <t>C208</t>
+  </si>
+  <si>
+    <t>C209</t>
+  </si>
+  <si>
+    <t>C210</t>
+  </si>
+  <si>
+    <t>C211</t>
+  </si>
+  <si>
+    <t>C212</t>
+  </si>
+  <si>
+    <t>C213</t>
+  </si>
+  <si>
+    <t>C214</t>
+  </si>
+  <si>
+    <t>C215</t>
+  </si>
+  <si>
+    <t>C216</t>
+  </si>
+  <si>
+    <t>C217</t>
+  </si>
+  <si>
+    <t>C218</t>
+  </si>
+  <si>
+    <t>C219</t>
+  </si>
+  <si>
+    <t>C220</t>
+  </si>
+  <si>
+    <t>C221</t>
+  </si>
+  <si>
+    <t>C222</t>
+  </si>
+  <si>
+    <t>C223</t>
+  </si>
+  <si>
+    <t>C224</t>
+  </si>
+  <si>
+    <t>C225</t>
+  </si>
+  <si>
+    <t>C226</t>
+  </si>
+  <si>
+    <t>C227</t>
+  </si>
+  <si>
+    <t>C228</t>
+  </si>
+  <si>
+    <t>C229</t>
+  </si>
+  <si>
+    <t>C230</t>
+  </si>
+  <si>
+    <t>C231</t>
+  </si>
+  <si>
+    <t>C232</t>
+  </si>
+  <si>
+    <t>C233</t>
+  </si>
+  <si>
+    <t>C234</t>
+  </si>
+  <si>
+    <t>C235</t>
+  </si>
+  <si>
+    <t>C236</t>
+  </si>
+  <si>
+    <t>C237</t>
+  </si>
+  <si>
+    <t>C238</t>
+  </si>
+  <si>
+    <t>C239</t>
+  </si>
+  <si>
+    <t>C240</t>
+  </si>
+  <si>
+    <t>C241</t>
+  </si>
+  <si>
+    <t>C242</t>
+  </si>
+  <si>
+    <t>C243</t>
+  </si>
+  <si>
+    <t>C244</t>
+  </si>
+  <si>
+    <t>C245</t>
+  </si>
+  <si>
+    <t>C246</t>
+  </si>
+  <si>
+    <t>C247</t>
+  </si>
+  <si>
+    <t>C248</t>
+  </si>
+  <si>
+    <t>C249</t>
+  </si>
+  <si>
+    <t>C250</t>
+  </si>
+  <si>
+    <t>C251</t>
+  </si>
+  <si>
+    <t>C252</t>
+  </si>
+  <si>
+    <t>C253</t>
+  </si>
+  <si>
+    <t>C254</t>
+  </si>
+  <si>
+    <t>C255</t>
+  </si>
+  <si>
+    <t>C256</t>
+  </si>
+  <si>
+    <t>C257</t>
+  </si>
+  <si>
+    <t>C258</t>
+  </si>
+  <si>
+    <t>C259</t>
+  </si>
+  <si>
+    <t>C260</t>
+  </si>
+  <si>
+    <t>C261</t>
+  </si>
+  <si>
+    <t>C262</t>
+  </si>
+  <si>
+    <t>C263</t>
+  </si>
+  <si>
+    <t>C264</t>
+  </si>
+  <si>
+    <t>C265</t>
+  </si>
+  <si>
+    <t>C266</t>
+  </si>
+  <si>
+    <t>C267</t>
+  </si>
+  <si>
+    <t>C268</t>
+  </si>
+  <si>
+    <t>C269</t>
+  </si>
+  <si>
+    <t>C270</t>
+  </si>
+  <si>
+    <t>C271</t>
+  </si>
+  <si>
+    <t>C272</t>
+  </si>
+  <si>
+    <t>C273</t>
+  </si>
+  <si>
+    <t>C274</t>
+  </si>
+  <si>
+    <t>C275</t>
+  </si>
+  <si>
+    <t>C276</t>
+  </si>
+  <si>
+    <t>C277</t>
+  </si>
+  <si>
+    <t>C278</t>
+  </si>
+  <si>
+    <t>C279</t>
+  </si>
+  <si>
+    <t>C280</t>
+  </si>
+  <si>
+    <t>C281</t>
+  </si>
+  <si>
+    <t>C282</t>
+  </si>
+  <si>
+    <t>C283</t>
+  </si>
+  <si>
+    <t>C284</t>
+  </si>
+  <si>
+    <t>C285</t>
+  </si>
+  <si>
+    <t>C286</t>
+  </si>
+  <si>
+    <t>C287</t>
+  </si>
+  <si>
+    <t>C288</t>
+  </si>
+  <si>
+    <t>C289</t>
+  </si>
+  <si>
+    <t>C290</t>
+  </si>
+  <si>
+    <t>C291</t>
+  </si>
+  <si>
+    <t>C292</t>
+  </si>
+  <si>
+    <t>C293</t>
+  </si>
+  <si>
+    <t>C294</t>
+  </si>
+  <si>
+    <t>C295</t>
+  </si>
+  <si>
+    <t>C296</t>
+  </si>
+  <si>
+    <t>C297</t>
+  </si>
+  <si>
+    <t>C298</t>
+  </si>
+  <si>
+    <t>C299</t>
+  </si>
+  <si>
+    <t>C300</t>
+  </si>
+  <si>
+    <t>C301</t>
+  </si>
+  <si>
+    <t>C302</t>
+  </si>
+  <si>
+    <t>C303</t>
+  </si>
+  <si>
+    <t>C304</t>
+  </si>
+  <si>
+    <t>C305</t>
+  </si>
+  <si>
+    <t>C306</t>
+  </si>
+  <si>
+    <t>C307</t>
+  </si>
+  <si>
+    <t>C308</t>
+  </si>
+  <si>
+    <t>C309</t>
+  </si>
+  <si>
+    <t>C310</t>
+  </si>
+  <si>
+    <t>C311</t>
+  </si>
+  <si>
+    <t>C312</t>
+  </si>
+  <si>
+    <t>C313</t>
+  </si>
+  <si>
+    <t>C314</t>
   </si>
 </sst>
 </file>
@@ -1475,10 +2255,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:C315"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1880,6 +2660,1306 @@
         <v>200</v>
       </c>
     </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="4" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="4" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="4" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="4" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="4" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="4" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="4" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="4" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="4" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="4" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="4" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="4" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="4" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="4" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="4" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="4" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="4" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="4" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="4" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="4" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="4" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="4" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="4" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="4" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="4" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="4" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="4" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="4" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="4" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="4" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="4" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="4" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="4" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="4" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="4" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="4" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="4" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="4" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="4" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="4" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="4" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="4" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="4" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="4" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="4" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="4" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="4" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="4" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="4" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="4" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="4" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="4" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="4" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="4" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="4" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="4" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="4" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="4" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" s="4" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" s="4" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="4" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" s="4" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="4" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="4" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" s="4" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="4" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" s="4" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" s="4" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" s="4" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" s="4" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" s="4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" s="4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" s="4" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" s="4" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" s="4" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" s="4" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="4" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="4" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="4" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="4" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" s="4" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="4" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="4" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" s="4" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" s="4" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="4" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" s="4" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="4" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" s="4" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" s="4" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" s="4" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" s="4" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" s="4" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" s="4" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" s="4" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" s="4" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" s="4" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" s="4" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" s="4" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" s="4" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" s="4" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" s="4" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" s="4" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" s="4" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" s="4" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" s="4" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" s="4" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" s="4" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209" s="4" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210" s="4" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211" s="4" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" s="4" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" s="4" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" s="4" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215" s="4" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216" s="4" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217" s="4" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218" s="4" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A219" s="4" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220" s="4" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221" s="4" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222" s="4" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A223" s="4" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224" s="4" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225" s="4" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226" s="4" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227" s="4" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228" s="4" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229" s="4" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230" s="4" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231" s="4" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232" s="4" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233" s="4" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234" s="4" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235" s="4" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A236" s="4" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237" s="4" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A238" s="4" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A239" s="4" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A240" s="4" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A241" s="4" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A242" s="4" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A243" s="4" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A244" s="4" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A245" s="4" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A246" s="4" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A247" s="4" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A248" s="4" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A249" s="4" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A250" s="4" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A251" s="4" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A252" s="4" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A253" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A254" s="4" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A255" s="4" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A256" s="4" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A257" s="4" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A258" s="4" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A259" s="4" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A260" s="4" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A261" s="4" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A262" s="4" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A263" s="4" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A264" s="4" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A265" s="4" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A266" s="4" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A267" s="4" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A268" s="4" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A269" s="4" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A270" s="4" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A271" s="4" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A272" s="4" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A273" s="4" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A274" s="4" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A275" s="4" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A276" s="4" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A277" s="4" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A278" s="4" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A279" s="4" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A280" s="4" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A281" s="4" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A282" s="4" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A283" s="4" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A284" s="4" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A285" s="4" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A286" s="4" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A287" s="4" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A288" s="4" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A289" s="4" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A290" s="4" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A291" s="4" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A292" s="4" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A293" s="4" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A294" s="4" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A295" s="4" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A296" s="4" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A297" s="4" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A298" s="4" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A299" s="4" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A300" s="4" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A301" s="4" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A302" s="4" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A303" s="4" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A304" s="4" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A305" s="4" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A306" s="4" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A307" s="4" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A308" s="4" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A309" s="4" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A310" s="4" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A311" s="4" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A312" s="4" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A313" s="4" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A314" s="4" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A315" s="4" t="s">
+        <v>465</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1889,7 +3969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
@@ -4796,8 +6876,8 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Finish creditQ delta and vega
</commit_message>
<xml_diff>
--- a/simm_config.xlsx
+++ b/simm_config.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="529">
   <si>
     <t>curr</t>
   </si>
@@ -501,9 +501,6 @@
     <t>Include</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>S_IR_8,S_IR_9</t>
   </si>
   <si>
@@ -1552,6 +1549,66 @@
   </si>
   <si>
     <t>All S_CRQ</t>
+  </si>
+  <si>
+    <t>S_CRV_1</t>
+  </si>
+  <si>
+    <t>Risk_CreditVol</t>
+  </si>
+  <si>
+    <t>US.IG</t>
+  </si>
+  <si>
+    <t>S_CRV_2</t>
+  </si>
+  <si>
+    <t>EU.HY</t>
+  </si>
+  <si>
+    <t>S_CRV_3</t>
+  </si>
+  <si>
+    <t>S_CRV_4</t>
+  </si>
+  <si>
+    <t>S_CRV_5</t>
+  </si>
+  <si>
+    <t>S_CRV_6</t>
+  </si>
+  <si>
+    <t>US.XX</t>
+  </si>
+  <si>
+    <t>S_CRV_7</t>
+  </si>
+  <si>
+    <t>CN.HY</t>
+  </si>
+  <si>
+    <t>S_CRV_8</t>
+  </si>
+  <si>
+    <t>S_CRV_1, S_CRV_3</t>
+  </si>
+  <si>
+    <t>S_CRV_2, S_CRV_5</t>
+  </si>
+  <si>
+    <t>S_CRV_4, S_CRV_5</t>
+  </si>
+  <si>
+    <t>S_CRV_2, S_CRV_4</t>
+  </si>
+  <si>
+    <t>S_CRV_1, S_CRV_6</t>
+  </si>
+  <si>
+    <t>S_CRV_7, S_CRV_8</t>
+  </si>
+  <si>
+    <t>All S_CRV</t>
   </si>
 </sst>
 </file>
@@ -2389,8 +2446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C315"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
+      <selection activeCell="C177" sqref="C177:C183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2584,7 +2641,7 @@
         <v>143</v>
       </c>
       <c r="B23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -2592,7 +2649,7 @@
         <v>149</v>
       </c>
       <c r="B24" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -2608,7 +2665,7 @@
         <v>151</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -2616,7 +2673,7 @@
         <v>152</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -2624,7 +2681,7 @@
         <v>153</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -2632,7 +2689,7 @@
         <v>154</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -2640,7 +2697,7 @@
         <v>155</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -2648,7 +2705,7 @@
         <v>156</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -2656,68 +2713,68 @@
         <v>157</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B37" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B38" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B39" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>77</v>
@@ -2725,7 +2782,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>81</v>
@@ -2733,579 +2790,576 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="B48" s="4" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
+      <c r="B49" s="4" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B50" s="4" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="B50" s="4" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
+      <c r="B60" s="4" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B61" s="4" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="B62" s="4" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B63" s="4" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B64" s="4" t="s">
         <v>499</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>500</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B87" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B142" s="4" t="s">
         <v>106</v>
@@ -3313,7 +3367,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B143" s="4" t="s">
         <v>108</v>
@@ -3321,7 +3375,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B144" s="4" t="s">
         <v>109</v>
@@ -3329,7 +3383,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B145" s="4" t="s">
         <v>110</v>
@@ -3337,7 +3391,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B146" s="4" t="s">
         <v>111</v>
@@ -3345,7 +3399,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B147" s="4" t="s">
         <v>112</v>
@@ -3353,7 +3407,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B148" s="4" t="s">
         <v>113</v>
@@ -3361,7 +3415,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B149" s="4" t="s">
         <v>114</v>
@@ -3369,889 +3423,934 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B150" s="4" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B155" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B158" s="4" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B161" s="4" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B162" s="4" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B164" s="4" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B165" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B166" s="4" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B167" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B168" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
+      </c>
+      <c r="B169" s="4" t="s">
+        <v>509</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
+      </c>
+      <c r="B170" s="4" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
+      </c>
+      <c r="B171" s="4" t="s">
+        <v>514</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
+      </c>
+      <c r="B172" s="4" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
+      </c>
+      <c r="B173" s="4" t="s">
+        <v>516</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
+      </c>
+      <c r="B174" s="4" t="s">
+        <v>517</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
+      </c>
+      <c r="B175" s="4" t="s">
+        <v>519</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="B176" s="4" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" s="4" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A177" s="4" t="s">
+      <c r="B177" s="4" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" s="4" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A178" s="4" t="s">
+      <c r="B178" s="4" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" s="4" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A179" s="4" t="s">
+      <c r="B179" s="4" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180" s="4" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A180" s="4" t="s">
+      <c r="B180" s="4" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181" s="4" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A181" s="4" t="s">
+      <c r="B181" s="4" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182" s="4" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A182" s="4" t="s">
+      <c r="B182" s="4" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183" s="4" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A183" s="4" t="s">
+      <c r="B183" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" s="4" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A184" s="4" t="s">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185" s="4" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A185" s="4" t="s">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" s="4" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A186" s="4" t="s">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187" s="4" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A187" s="4" t="s">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188" s="4" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A188" s="4" t="s">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189" s="4" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A189" s="4" t="s">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" s="4" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A190" s="4" t="s">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" s="4" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A191" s="4" t="s">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" s="4" t="s">
         <v>331</v>
-      </c>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A192" s="4" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" s="4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A202" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A203" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A204" s="4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205" s="4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A206" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A207" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A208" s="4" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A209" s="4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A210" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A211" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A212" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A213" s="4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A214" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A215" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A216" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A217" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A218" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A219" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A220" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A221" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A222" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A223" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A224" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A225" s="4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A226" s="4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A227" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A228" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A229" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A230" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A231" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A232" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A233" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A234" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A235" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A236" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A237" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A238" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A239" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A240" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A241" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A242" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A243" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A244" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A245" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A246" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A247" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A248" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A249" s="4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A250" s="4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A251" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A252" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A253" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A254" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A255" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A256" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A257" s="4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A258" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A259" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A260" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A261" s="4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A262" s="4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A263" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A264" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A265" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A266" s="4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A267" s="4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A268" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A269" s="4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A270" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A271" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A272" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A273" s="4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A274" s="4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A275" s="4" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A276" s="4" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A277" s="4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A278" s="4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A279" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A280" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A281" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A282" s="4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A283" s="4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A284" s="4" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A285" s="4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A286" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A287" s="4" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A288" s="4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A289" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A290" s="4" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A291" s="4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A292" s="4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A293" s="4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A294" s="4" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A295" s="4" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A296" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A297" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A298" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="299" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A299" s="4" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="300" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A300" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="301" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A301" s="4" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="302" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A302" s="4" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="303" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A303" s="4" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="304" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A304" s="4" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="305" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A305" s="4" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="306" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A306" s="4" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="307" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A307" s="4" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="308" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A308" s="4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="309" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A309" s="4" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="310" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A310" s="4" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="311" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A311" s="4" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="312" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A312" s="4" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="313" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A313" s="4" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="314" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A314" s="4" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="315" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A315" s="4" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
   </sheetData>
@@ -4261,10 +4360,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J61"/>
+  <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:B28"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56:B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4273,6 +4372,8 @@
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -4831,7 +4932,7 @@
         <v>51</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="H19" s="4">
         <v>-1000000</v>
@@ -4848,13 +4949,13 @@
         <v>97</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>78</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E20" s="4">
         <v>2</v>
@@ -4863,7 +4964,7 @@
         <v>54</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="H20" s="4">
         <v>2000000</v>
@@ -4880,13 +4981,13 @@
         <v>97</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>78</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E21" s="4">
         <v>2</v>
@@ -4909,13 +5010,13 @@
         <v>97</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>78</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E22" s="4">
         <v>5</v>
@@ -4938,13 +5039,13 @@
         <v>97</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>78</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E23" s="4">
         <v>5</v>
@@ -4967,13 +5068,13 @@
         <v>97</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>78</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E24" s="4">
         <v>7</v>
@@ -4996,13 +5097,13 @@
         <v>97</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>78</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E25" s="4">
         <v>7</v>
@@ -5025,13 +5126,13 @@
         <v>97</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>78</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E26" s="4">
         <v>9</v>
@@ -5054,7 +5155,7 @@
         <v>97</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>78</v>
@@ -5083,13 +5184,13 @@
         <v>97</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>78</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>21</v>
@@ -5728,183 +5829,416 @@
         <v>-100000000</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="4"/>
-      <c r="B55" s="4"/>
-      <c r="C55" s="4"/>
-      <c r="D55" s="4"/>
-      <c r="E55" s="4"/>
-      <c r="F55" s="4"/>
-      <c r="G55" s="4"/>
-      <c r="H55" s="4"/>
-      <c r="I55" s="4"/>
-      <c r="J55" s="4"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>468</v>
+        <v>509</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>115</v>
+        <v>510</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E56" s="4"/>
+        <v>511</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F56" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G56" s="4"/>
+        <v>54</v>
+      </c>
       <c r="H56" s="4">
-        <v>10000000</v>
+        <v>200000000</v>
       </c>
       <c r="I56" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J56" s="4">
-        <v>10000000</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+        <v>200000000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>469</v>
+        <v>512</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>115</v>
+        <v>510</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E57" s="4"/>
+        <v>513</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F57" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G57" s="4"/>
+        <v>54</v>
+      </c>
       <c r="H57" s="4">
-        <v>-50000000</v>
+        <v>-500000000</v>
       </c>
       <c r="I57" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J57" s="4">
-        <v>-50000000</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+        <v>-500000000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>470</v>
+        <v>514</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>115</v>
+        <v>510</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="E58" s="4"/>
+        <v>511</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F58" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="G58" s="4"/>
       <c r="H58" s="4">
-        <v>4500000</v>
+        <v>300000000</v>
       </c>
       <c r="I58" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J58" s="4">
-        <v>4500000</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+        <v>300000000</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>471</v>
+        <v>515</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>115</v>
+        <v>510</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="E59" s="4"/>
+        <v>513</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F59" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G59" s="4"/>
+        <v>80</v>
+      </c>
       <c r="H59" s="4">
-        <v>20000000</v>
+        <v>200000000</v>
       </c>
       <c r="I59" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J59" s="4">
-        <v>20000000</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+        <v>200000000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>472</v>
+        <v>516</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>115</v>
+        <v>510</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="E60" s="4"/>
+        <v>513</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F60" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G60" s="4"/>
+        <v>80</v>
+      </c>
       <c r="H60" s="4">
-        <v>-10000000</v>
+        <v>-100000000</v>
       </c>
       <c r="I60" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J60" s="4">
-        <v>-10000000</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+        <v>-100000000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>473</v>
+        <v>517</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>115</v>
+        <v>510</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="E61" s="4"/>
+        <v>518</v>
+      </c>
+      <c r="E61" s="4">
+        <v>1</v>
+      </c>
       <c r="F61" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="G61" s="4"/>
       <c r="H61" s="4">
-        <v>90000000</v>
+        <v>300000000</v>
       </c>
       <c r="I61" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J61" s="4">
+        <v>300000000</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>519</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>510</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>520</v>
+      </c>
+      <c r="E62" s="4">
+        <v>2</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H62" s="4">
+        <v>250000000</v>
+      </c>
+      <c r="I62" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J62" s="4">
+        <v>250000000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>521</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>510</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>520</v>
+      </c>
+      <c r="E63" s="4">
+        <v>2</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H63" s="4">
+        <v>-200000000</v>
+      </c>
+      <c r="I63" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J63" s="4">
+        <v>-200000000</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
+      <c r="H64" s="4"/>
+      <c r="I64" s="4"/>
+      <c r="J64" s="4"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G65" s="4"/>
+      <c r="H65" s="4">
+        <v>10000000</v>
+      </c>
+      <c r="I65" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J65" s="4">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>468</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E66" s="4"/>
+      <c r="F66" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G66" s="4"/>
+      <c r="H66" s="4">
+        <v>-50000000</v>
+      </c>
+      <c r="I66" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J66" s="4">
+        <v>-50000000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>469</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E67" s="4"/>
+      <c r="F67" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G67" s="4"/>
+      <c r="H67" s="4">
+        <v>4500000</v>
+      </c>
+      <c r="I67" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J67" s="4">
+        <v>4500000</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E68" s="4"/>
+      <c r="F68" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G68" s="4"/>
+      <c r="H68" s="4">
+        <v>20000000</v>
+      </c>
+      <c r="I68" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J68" s="4">
+        <v>20000000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E69" s="4"/>
+      <c r="F69" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G69" s="4"/>
+      <c r="H69" s="4">
+        <v>-10000000</v>
+      </c>
+      <c r="I69" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J69" s="4">
+        <v>-10000000</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>472</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E70" s="4"/>
+      <c r="F70" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G70" s="4"/>
+      <c r="H70" s="4">
+        <v>90000000</v>
+      </c>
+      <c r="I70" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J70" s="4">
         <v>90000000</v>
       </c>
     </row>
@@ -6778,7 +7112,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7436,7 +7770,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7458,7 +7792,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B2" s="4">
         <v>1000000</v>
@@ -7469,7 +7803,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B3" s="4">
         <v>360000</v>
@@ -7480,7 +7814,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B4" s="4">
         <v>360000</v>

</xml_diff>

<commit_message>
Finish Equity Delta. Have issue with Equity Vega
</commit_message>
<xml_diff>
--- a/simm_config.xlsx
+++ b/simm_config.xlsx
@@ -18,14 +18,18 @@
     <sheet name="CreditNonQ_weights" sheetId="11" r:id="rId9"/>
     <sheet name="CreditNonQ_correlation" sheetId="12" r:id="rId10"/>
     <sheet name="CreditNonQ_CR_THR" sheetId="13" r:id="rId11"/>
-    <sheet name="FX_CR_THR" sheetId="8" r:id="rId12"/>
+    <sheet name="Equity_weights" sheetId="14" r:id="rId12"/>
+    <sheet name="Equity_correlation" sheetId="15" r:id="rId13"/>
+    <sheet name="Equity_in_bucket_correlation" sheetId="16" r:id="rId14"/>
+    <sheet name="Equity_CR_THR" sheetId="17" r:id="rId15"/>
+    <sheet name="FX_CR_THR" sheetId="8" r:id="rId16"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="632">
   <si>
     <t>curr</t>
   </si>
@@ -1765,6 +1769,162 @@
   </si>
   <si>
     <t>All S_CNV</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>corr</t>
+  </si>
+  <si>
+    <t>Emerging Markets - Large Cap</t>
+  </si>
+  <si>
+    <t>Developed Markets - Large Cap</t>
+  </si>
+  <si>
+    <t>Emerging Markets - Small Cap</t>
+  </si>
+  <si>
+    <t>Developed Markets - Small Cap</t>
+  </si>
+  <si>
+    <t>Indexeds, Funds, ETFs</t>
+  </si>
+  <si>
+    <t>S_EQ_3</t>
+  </si>
+  <si>
+    <t>ISIN:AT0000743059</t>
+  </si>
+  <si>
+    <t>S_EQ_4</t>
+  </si>
+  <si>
+    <t>ISIN:AU000000GMG2</t>
+  </si>
+  <si>
+    <t>S_EQ_5</t>
+  </si>
+  <si>
+    <t>ISIN:AU000000GPT8</t>
+  </si>
+  <si>
+    <t>S_EQ_6</t>
+  </si>
+  <si>
+    <t>ISIN:AT0000606306</t>
+  </si>
+  <si>
+    <t>S_EQ_7</t>
+  </si>
+  <si>
+    <t>ISIN:BMG702781094</t>
+  </si>
+  <si>
+    <t>S_EQ_8</t>
+  </si>
+  <si>
+    <t>ISIN:BRCSMGACNOR5</t>
+  </si>
+  <si>
+    <t>S_EQ_9</t>
+  </si>
+  <si>
+    <t>ISIN:CA37989N1069</t>
+  </si>
+  <si>
+    <t>S_EQ_10</t>
+  </si>
+  <si>
+    <t>SPX</t>
+  </si>
+  <si>
+    <t>S_EQ_11</t>
+  </si>
+  <si>
+    <t>ISIN:AT0000697750</t>
+  </si>
+  <si>
+    <t>S_EQ_13</t>
+  </si>
+  <si>
+    <t>S_EQ_4, S_EQ_5</t>
+  </si>
+  <si>
+    <t>S_EQ_12, S_EQ_13</t>
+  </si>
+  <si>
+    <t>S_EQ_4, S_EQ_6</t>
+  </si>
+  <si>
+    <t>S_EQ_1, S_EQ_3</t>
+  </si>
+  <si>
+    <t>S_EQ_8, S_EQ_9</t>
+  </si>
+  <si>
+    <t>S_EQ_8, S_EQ_13</t>
+  </si>
+  <si>
+    <t>S_EQ_5, S_EQ_6, S_EQ_7</t>
+  </si>
+  <si>
+    <t>S_EQ_7, S_EQ_9, S_EQ_10</t>
+  </si>
+  <si>
+    <t>S_EQ_4, S_EQ_5, S_EQ_11</t>
+  </si>
+  <si>
+    <t>S_EQ_5, S_EQ_10, S_EQ_11</t>
+  </si>
+  <si>
+    <t>All S_EQ</t>
+  </si>
+  <si>
+    <t>S_EQ_2, S_EQ_3</t>
+  </si>
+  <si>
+    <t>S_EQV_1</t>
+  </si>
+  <si>
+    <t>S_EQV_2</t>
+  </si>
+  <si>
+    <t>S_EQV_3</t>
+  </si>
+  <si>
+    <t>S_EQV_4</t>
+  </si>
+  <si>
+    <t>S_EQV_5</t>
+  </si>
+  <si>
+    <t>S_EQV_6</t>
+  </si>
+  <si>
+    <t>ISIN:AT0000912345</t>
+  </si>
+  <si>
+    <t>Risk_EquityVol</t>
+  </si>
+  <si>
+    <t>S_EQV_1, S_EQV_3</t>
+  </si>
+  <si>
+    <t>S_EQV_2, S_EQV_5</t>
+  </si>
+  <si>
+    <t>S_EQV_4, S_EQV_5</t>
+  </si>
+  <si>
+    <t>S_EQV_2, S_EQV_3</t>
+  </si>
+  <si>
+    <t>S_EQV_1, S_EQV_6</t>
+  </si>
+  <si>
+    <t>All S_EQV</t>
   </si>
 </sst>
 </file>
@@ -2602,8 +2762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C315"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A197" workbookViewId="0">
+      <selection activeCell="C206" sqref="C206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2632,7 +2792,7 @@
         <v>45</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>159</v>
+        <v>580</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3335,193 +3495,268 @@
       <c r="A90" s="4" t="s">
         <v>230</v>
       </c>
+      <c r="B90" s="4" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>231</v>
       </c>
+      <c r="B91" s="4" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>232</v>
       </c>
+      <c r="B92" s="4" t="s">
+        <v>587</v>
+      </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>233</v>
       </c>
+      <c r="B93" s="4" t="s">
+        <v>589</v>
+      </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>234</v>
       </c>
+      <c r="B94" s="4" t="s">
+        <v>591</v>
+      </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>235</v>
       </c>
+      <c r="B95" s="4" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B96" s="4" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B97" s="4" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B98" s="4" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B99" s="4" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B100" s="4" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B101" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B102" s="4" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B103" s="4" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B104" s="4" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B105" s="4" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B106" s="4" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B107" s="4" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B108" s="4" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B109" s="4" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B110" s="4" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B111" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B112" s="4" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B113" s="4" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
         <v>268</v>
       </c>
@@ -3999,7 +4234,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="4" t="s">
         <v>333</v>
       </c>
@@ -4007,7 +4242,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="4" t="s">
         <v>334</v>
       </c>
@@ -4015,7 +4250,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="4" t="s">
         <v>335</v>
       </c>
@@ -4023,7 +4258,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="4" t="s">
         <v>336</v>
       </c>
@@ -4031,7 +4266,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="4" t="s">
         <v>337</v>
       </c>
@@ -4039,7 +4274,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="4" t="s">
         <v>338</v>
       </c>
@@ -4047,132 +4282,171 @@
         <v>579</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="4" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B199" s="4" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="4" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B200" s="4" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" s="4" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B201" s="4" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" s="4" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B202" s="4" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" s="4" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B203" s="4" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" s="4" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B204" s="4" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" s="4" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B205" s="4" t="s">
+        <v>626</v>
+      </c>
+      <c r="C205" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" s="4" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B206" s="4" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" s="4" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B207" s="4" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" s="4" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B208" s="4" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" s="4" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B209" s="4" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" s="4" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B210" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" s="4" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" s="4" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" s="4" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" s="4" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" s="4" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" s="4" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" s="4" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" s="4" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" s="4" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" s="4" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" s="4" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" s="4" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" s="4" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" s="4" t="s">
         <v>364</v>
       </c>
@@ -4687,7 +4961,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4756,6 +5030,868 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF7030A0"/>
+  </sheetPr>
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>28.000000000000004</v>
+      </c>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>28.000000000000004</v>
+      </c>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>25</v>
+      </c>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>18</v>
+      </c>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4">
+        <v>20</v>
+      </c>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4">
+        <v>24</v>
+      </c>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4">
+        <v>23</v>
+      </c>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4">
+        <v>26</v>
+      </c>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4">
+        <v>27</v>
+      </c>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4">
+        <v>15</v>
+      </c>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="4">
+        <v>28.000000000000004</v>
+      </c>
+      <c r="D13" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF7030A0"/>
+  </sheetPr>
+  <dimension ref="A1:K13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="4">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4">
+        <v>3</v>
+      </c>
+      <c r="D1" s="4">
+        <v>4</v>
+      </c>
+      <c r="E1" s="4">
+        <v>5</v>
+      </c>
+      <c r="F1" s="4">
+        <v>6</v>
+      </c>
+      <c r="G1" s="4">
+        <v>7</v>
+      </c>
+      <c r="H1" s="4">
+        <v>8</v>
+      </c>
+      <c r="I1" s="4">
+        <v>9</v>
+      </c>
+      <c r="J1" s="4">
+        <v>10</v>
+      </c>
+      <c r="K1" s="4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.17</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.18</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.16</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0.16</v>
+      </c>
+      <c r="J2" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="K2" s="4">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>0.17</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.24</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.19</v>
+      </c>
+      <c r="E3" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0.09</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I3" s="4">
+        <v>0.19</v>
+      </c>
+      <c r="J3" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K3" s="4">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>0.18</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.24</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.21</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.09</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0.13</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0.13</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="K4" s="4">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>0.16</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.19</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.21</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.13</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.17</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0.16</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0.17</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0.13</v>
+      </c>
+      <c r="K5" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="B6" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.09</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.13</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0.24</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="I6" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0.23</v>
+      </c>
+      <c r="K6" s="4">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.17</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0.33</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0.13</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0.26</v>
+      </c>
+      <c r="K7" s="4">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.09</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.13</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.16</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.24</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="G8" s="4">
+        <v>1</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="I8" s="4">
+        <v>0.13</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="K8" s="4">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.13</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.17</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0.33</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H9" s="4">
+        <v>1</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0.27</v>
+      </c>
+      <c r="K9" s="4">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>0.16</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.19</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.13</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0.13</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="I10" s="4">
+        <v>1</v>
+      </c>
+      <c r="J10" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="K10" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.13</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0.23</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0.26</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0.27</v>
+      </c>
+      <c r="I11" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="J11" s="4">
+        <v>1</v>
+      </c>
+      <c r="K11" s="4">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>0.18</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0.18</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.24</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0.38</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0.45</v>
+      </c>
+      <c r="G12" s="4">
+        <v>0.42</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0.45</v>
+      </c>
+      <c r="I12" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0.34</v>
+      </c>
+      <c r="K12" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF7030A0"/>
+  </sheetPr>
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF7030A0"/>
+  </sheetPr>
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>582</v>
+      </c>
+      <c r="B2" s="4">
+        <v>3100000</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>583</v>
+      </c>
+      <c r="B3" s="4">
+        <v>31000000</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>584</v>
+      </c>
+      <c r="B4" s="4">
+        <v>700000</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>585</v>
+      </c>
+      <c r="B5" s="4">
+        <v>2100000</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>586</v>
+      </c>
+      <c r="B6" s="4">
+        <v>690000000</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>481</v>
+      </c>
+      <c r="B7" s="4">
+        <v>700000</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>582</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1100000000</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>583</v>
+      </c>
+      <c r="B9" s="4">
+        <v>11000000000</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>584</v>
+      </c>
+      <c r="B10" s="4">
+        <v>170000000</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>585</v>
+      </c>
+      <c r="B11" s="4">
+        <v>500000000</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>586</v>
+      </c>
+      <c r="B12" s="4">
+        <v>39000000000</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>481</v>
+      </c>
+      <c r="B13" s="4">
+        <v>170000000</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
@@ -4868,10 +6004,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J88"/>
+  <dimension ref="A1:J106"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74:B81"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="E102" sqref="E102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5978,297 +7114,300 @@
         <v>-1000000</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-    </row>
+    <row r="39" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E40" s="4"/>
+        <v>94</v>
+      </c>
+      <c r="E40" s="4">
+        <v>6</v>
+      </c>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
       <c r="H40" s="4">
-        <v>1000000000</v>
+        <v>20000000</v>
       </c>
       <c r="I40" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J40" s="4">
-        <v>1000000000</v>
+        <v>20000000</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E41" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="E41" s="4">
+        <v>7</v>
+      </c>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
       <c r="H41" s="4">
-        <v>-1000000000</v>
+        <v>-40000000</v>
       </c>
       <c r="I41" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J41" s="4">
-        <v>-1000000000</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+        <v>-40000000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>85</v>
+        <v>587</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
+        <v>588</v>
+      </c>
+      <c r="E42" s="4">
+        <v>7</v>
+      </c>
       <c r="H42" s="4">
-        <v>-1500000000</v>
+        <v>10000000</v>
       </c>
       <c r="I42" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J42" s="4">
-        <v>-1500000000</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>86</v>
+        <v>589</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
+        <v>590</v>
+      </c>
+      <c r="E43" s="4">
+        <v>3</v>
+      </c>
       <c r="H43" s="4">
-        <v>1500000000</v>
+        <v>5000000</v>
       </c>
       <c r="I43" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J43" s="4">
-        <v>1500000000</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>87</v>
+        <v>591</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
+        <v>592</v>
+      </c>
+      <c r="E44" s="4">
+        <v>3</v>
+      </c>
       <c r="H44" s="4">
-        <v>6000000000</v>
+        <v>2000000</v>
       </c>
       <c r="I44" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J44" s="4">
-        <v>6000000000</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>88</v>
+        <v>593</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
+        <v>594</v>
+      </c>
+      <c r="E45" s="4">
+        <v>3</v>
+      </c>
       <c r="H45" s="4">
-        <v>-6000000000</v>
+        <v>10000000</v>
       </c>
       <c r="I45" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J45" s="4">
-        <v>-6000000000</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>89</v>
+        <v>595</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
+        <v>596</v>
+      </c>
+      <c r="E46" s="4">
+        <v>9</v>
+      </c>
       <c r="H46" s="4">
-        <v>-2300000000</v>
+        <v>1000000</v>
       </c>
       <c r="I46" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J46" s="4">
-        <v>-2300000000</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>90</v>
+        <v>597</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
+        <v>598</v>
+      </c>
+      <c r="E47" s="4">
+        <v>9</v>
+      </c>
       <c r="H47" s="4">
-        <v>2300000000</v>
+        <v>-2000000</v>
       </c>
       <c r="I47" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J47" s="4">
-        <v>2300000000</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="4"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+        <v>-2000000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>599</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>600</v>
+      </c>
+      <c r="E48" s="4">
+        <v>10</v>
+      </c>
+      <c r="H48" s="4">
+        <v>30000000</v>
+      </c>
+      <c r="I48" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J48" s="4">
+        <v>30000000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>76</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>92</v>
+        <v>601</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>93</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>94</v>
+        <v>602</v>
       </c>
       <c r="E49" s="4">
-        <v>6</v>
-      </c>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
+        <v>11</v>
+      </c>
       <c r="H49" s="4">
-        <v>20000</v>
+        <v>-40000000</v>
       </c>
       <c r="I49" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J49" s="4">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+        <v>-40000000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>76</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>95</v>
+        <v>603</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>93</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>96</v>
+        <v>604</v>
       </c>
       <c r="E50" s="4">
-        <v>7</v>
-      </c>
-      <c r="F50" s="4"/>
-      <c r="G50" s="4"/>
+        <v>10</v>
+      </c>
       <c r="H50" s="4">
-        <v>-40000</v>
+        <v>-4000000</v>
       </c>
       <c r="I50" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J50" s="4">
-        <v>-40000</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+        <v>-4000000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>98</v>
@@ -6282,124 +7421,130 @@
       <c r="E51" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F51" s="4"/>
-      <c r="G51" s="4"/>
       <c r="H51" s="4">
-        <v>20000</v>
+        <v>20000000</v>
       </c>
       <c r="I51" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J51" s="4">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="4"/>
-      <c r="B52" s="4"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="4"/>
-      <c r="F52" s="4"/>
-      <c r="G52" s="4"/>
-      <c r="H52" s="4"/>
-      <c r="I52" s="4"/>
-      <c r="J52" s="4"/>
+        <v>20000000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>605</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H52" s="4">
+        <v>-10000000</v>
+      </c>
+      <c r="I52" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J52" s="4">
+        <v>-10000000</v>
+      </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="E53" s="4">
-        <v>6</v>
-      </c>
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
       <c r="F53" s="4"/>
       <c r="G53" s="4"/>
-      <c r="H53" s="4">
-        <v>20000</v>
-      </c>
-      <c r="I53" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="J53" s="4">
-        <v>20000</v>
-      </c>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>100</v>
+        <v>44</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="E54" s="4">
-        <v>2</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="E54" s="4"/>
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
       <c r="H54" s="4">
-        <v>-40000</v>
+        <v>1000000000</v>
       </c>
       <c r="I54" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J54" s="4">
-        <v>-40000</v>
+        <v>1000000000</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="4"/>
-      <c r="B55" s="4"/>
-      <c r="C55" s="4"/>
-      <c r="D55" s="4"/>
+      <c r="A55" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
-      <c r="H55" s="4"/>
-      <c r="I55" s="4"/>
-      <c r="J55" s="4"/>
+      <c r="H55" s="4">
+        <v>-1000000000</v>
+      </c>
+      <c r="I55" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J55" s="4">
+        <v>-1000000000</v>
+      </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="E56" s="4"/>
-      <c r="F56" s="4" t="s">
-        <v>51</v>
-      </c>
+      <c r="F56" s="4"/>
       <c r="G56" s="4"/>
       <c r="H56" s="4">
-        <v>500000000</v>
+        <v>-1500000000</v>
       </c>
       <c r="I56" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J56" s="4">
-        <v>500000000</v>
+        <v>-1500000000</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
@@ -6407,27 +7552,25 @@
         <v>44</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="E57" s="4"/>
-      <c r="F57" s="4" t="s">
-        <v>54</v>
-      </c>
+      <c r="F57" s="4"/>
       <c r="G57" s="4"/>
       <c r="H57" s="4">
-        <v>-500000000</v>
+        <v>1500000000</v>
       </c>
       <c r="I57" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J57" s="4">
-        <v>-500000000</v>
+        <v>1500000000</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
@@ -6435,27 +7578,25 @@
         <v>44</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>63</v>
       </c>
       <c r="E58" s="4"/>
-      <c r="F58" s="4" t="s">
-        <v>80</v>
-      </c>
+      <c r="F58" s="4"/>
       <c r="G58" s="4"/>
       <c r="H58" s="4">
-        <v>300000000</v>
+        <v>6000000000</v>
       </c>
       <c r="I58" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J58" s="4">
-        <v>300000000</v>
+        <v>6000000000</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
@@ -6463,27 +7604,25 @@
         <v>44</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E59" s="4"/>
-      <c r="F59" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="F59" s="4"/>
       <c r="G59" s="4"/>
       <c r="H59" s="4">
-        <v>200000000</v>
+        <v>-6000000000</v>
       </c>
       <c r="I59" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J59" s="4">
-        <v>200000000</v>
+        <v>-6000000000</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
@@ -6491,27 +7630,25 @@
         <v>44</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E60" s="4"/>
-      <c r="F60" s="4" t="s">
-        <v>54</v>
-      </c>
+      <c r="F60" s="4"/>
       <c r="G60" s="4"/>
       <c r="H60" s="4">
-        <v>-100000000</v>
+        <v>-2300000000</v>
       </c>
       <c r="I60" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J60" s="4">
-        <v>-100000000</v>
+        <v>-2300000000</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
@@ -6519,388 +7656,353 @@
         <v>44</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>59</v>
+        <v>91</v>
       </c>
       <c r="E61" s="4"/>
-      <c r="F61" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="F61" s="4"/>
       <c r="G61" s="4"/>
       <c r="H61" s="4">
-        <v>20000000</v>
+        <v>2300000000</v>
       </c>
       <c r="I61" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J61" s="4">
-        <v>20000000</v>
+        <v>2300000000</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>72</v>
-      </c>
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
       <c r="E62" s="4"/>
-      <c r="F62" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="F62" s="4"/>
       <c r="G62" s="4"/>
-      <c r="H62" s="4">
-        <v>150000000</v>
-      </c>
-      <c r="I62" s="4" t="s">
+      <c r="H62" s="4"/>
+      <c r="I62" s="4"/>
+      <c r="J62" s="4"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="4"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
+      <c r="G63" s="4"/>
+      <c r="H63" s="4"/>
+      <c r="I63" s="4"/>
+      <c r="J63" s="4"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E64" s="4">
+        <v>6</v>
+      </c>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
+      <c r="H64" s="4">
+        <v>20000</v>
+      </c>
+      <c r="I64" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="J62" s="4">
-        <v>150000000</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="D63" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E63" s="4"/>
-      <c r="F63" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="G63" s="4"/>
-      <c r="H63" s="4">
-        <v>-100000000</v>
-      </c>
-      <c r="I63" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="J63" s="4">
-        <v>-100000000</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J64" s="4">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>510</v>
+        <v>104</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>511</v>
+        <v>102</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>512</v>
-      </c>
-      <c r="E65" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F65" s="4" t="s">
-        <v>54</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="E65" s="4">
+        <v>2</v>
+      </c>
+      <c r="F65" s="4"/>
+      <c r="G65" s="4"/>
       <c r="H65" s="4">
-        <v>200000000</v>
+        <v>-40000</v>
       </c>
       <c r="I65" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J65" s="4">
-        <v>200000000</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>513</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>511</v>
-      </c>
-      <c r="D66" s="4" t="s">
-        <v>514</v>
-      </c>
-      <c r="E66" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F66" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="H66" s="4">
-        <v>-500000000</v>
-      </c>
-      <c r="I66" s="4" t="s">
+        <v>-40000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" s="4"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
+      <c r="G66" s="4"/>
+      <c r="H66" s="4"/>
+      <c r="I66" s="4"/>
+      <c r="J66" s="4"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D67" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="J66" s="4">
-        <v>-500000000</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>515</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>511</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>512</v>
-      </c>
-      <c r="E67" s="4" t="s">
-        <v>21</v>
-      </c>
+      <c r="E67" s="4"/>
       <c r="F67" s="4" t="s">
-        <v>80</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="G67" s="4"/>
       <c r="H67" s="4">
-        <v>300000000</v>
+        <v>500000000</v>
       </c>
       <c r="I67" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J67" s="4">
-        <v>300000000</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>500000000</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>97</v>
+        <v>44</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>516</v>
+        <v>108</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>511</v>
+        <v>107</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>514</v>
-      </c>
-      <c r="E68" s="4" t="s">
-        <v>21</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="E68" s="4"/>
       <c r="F68" s="4" t="s">
-        <v>80</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="G68" s="4"/>
       <c r="H68" s="4">
-        <v>200000000</v>
+        <v>-500000000</v>
       </c>
       <c r="I68" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J68" s="4">
-        <v>200000000</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>-500000000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>97</v>
+        <v>44</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>517</v>
+        <v>109</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>511</v>
+        <v>107</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>514</v>
-      </c>
-      <c r="E69" s="4" t="s">
-        <v>21</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="E69" s="4"/>
       <c r="F69" s="4" t="s">
         <v>80</v>
       </c>
+      <c r="G69" s="4"/>
       <c r="H69" s="4">
-        <v>-100000000</v>
+        <v>300000000</v>
       </c>
       <c r="I69" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J69" s="4">
-        <v>-100000000</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>300000000</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>97</v>
+        <v>44</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>518</v>
+        <v>110</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>511</v>
+        <v>107</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>519</v>
-      </c>
-      <c r="E70" s="4">
-        <v>1</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="E70" s="4"/>
       <c r="F70" s="4" t="s">
-        <v>80</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="G70" s="4"/>
       <c r="H70" s="4">
-        <v>300000000</v>
+        <v>200000000</v>
       </c>
       <c r="I70" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J70" s="4">
-        <v>300000000</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>200000000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>97</v>
+        <v>44</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>520</v>
+        <v>111</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>511</v>
+        <v>107</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>521</v>
-      </c>
-      <c r="E71" s="4">
-        <v>2</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="E71" s="4"/>
       <c r="F71" s="4" t="s">
-        <v>80</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="G71" s="4"/>
       <c r="H71" s="4">
-        <v>250000000</v>
+        <v>-100000000</v>
       </c>
       <c r="I71" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J71" s="4">
-        <v>250000000</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>-100000000</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>97</v>
+        <v>44</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>522</v>
+        <v>112</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>511</v>
+        <v>107</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>521</v>
-      </c>
-      <c r="E72" s="4">
-        <v>2</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="E72" s="4"/>
       <c r="F72" s="4" t="s">
-        <v>54</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G72" s="4"/>
       <c r="H72" s="4">
-        <v>-200000000</v>
+        <v>20000000</v>
       </c>
       <c r="I72" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J72" s="4">
-        <v>-200000000</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>20000000</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E73" s="4"/>
+      <c r="F73" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G73" s="4"/>
+      <c r="H73" s="4">
+        <v>150000000</v>
+      </c>
+      <c r="I73" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J73" s="4">
+        <v>150000000</v>
+      </c>
+    </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>97</v>
+        <v>44</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>564</v>
+        <v>114</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>565</v>
+        <v>107</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>512</v>
-      </c>
-      <c r="E74" s="4" t="s">
-        <v>21</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="E74" s="4"/>
       <c r="F74" s="4" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="G74" s="4"/>
       <c r="H74" s="4">
-        <v>25000000</v>
+        <v>-100000000</v>
       </c>
       <c r="I74" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J74" s="4">
-        <v>25000000</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>566</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>565</v>
-      </c>
-      <c r="D75" s="4" t="s">
-        <v>514</v>
-      </c>
-      <c r="E75" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F75" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="G75" s="4"/>
-      <c r="H75" s="4">
-        <v>-60000000</v>
-      </c>
-      <c r="I75" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="J75" s="4">
-        <v>-60000000</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+        <v>-100000000</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>97</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>567</v>
+        <v>510</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>565</v>
+        <v>511</v>
       </c>
       <c r="D76" s="4" t="s">
         <v>512</v>
@@ -6909,28 +8011,27 @@
         <v>21</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="G76" s="4"/>
+        <v>54</v>
+      </c>
       <c r="H76" s="4">
-        <v>40000000</v>
+        <v>200000000</v>
       </c>
       <c r="I76" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J76" s="4">
-        <v>40000000</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+        <v>200000000</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>97</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>568</v>
+        <v>513</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>565</v>
+        <v>511</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>514</v>
@@ -6939,31 +8040,30 @@
         <v>21</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="G77" s="4"/>
+        <v>54</v>
+      </c>
       <c r="H77" s="4">
-        <v>30000000</v>
+        <v>-500000000</v>
       </c>
       <c r="I77" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J77" s="4">
-        <v>30000000</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+        <v>-500000000</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>97</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>569</v>
+        <v>515</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>565</v>
+        <v>511</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="E78" s="4" t="s">
         <v>21</v>
@@ -6971,284 +8071,754 @@
       <c r="F78" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="G78" s="4"/>
       <c r="H78" s="4">
-        <v>-15000000</v>
+        <v>300000000</v>
       </c>
       <c r="I78" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J78" s="4">
-        <v>-15000000</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+        <v>300000000</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>97</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>570</v>
+        <v>516</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>565</v>
+        <v>511</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>519</v>
-      </c>
-      <c r="E79" s="4">
-        <v>1</v>
+        <v>514</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="F79" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="G79" s="4"/>
       <c r="H79" s="4">
-        <v>60000000</v>
+        <v>200000000</v>
       </c>
       <c r="I79" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J79" s="4">
-        <v>60000000</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+        <v>200000000</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>97</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>571</v>
+        <v>517</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>565</v>
+        <v>511</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>521</v>
-      </c>
-      <c r="E80" s="4">
-        <v>2</v>
+        <v>514</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="F80" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="G80" s="4"/>
       <c r="H80" s="4">
-        <v>50000000</v>
+        <v>-100000000</v>
       </c>
       <c r="I80" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J80" s="4">
-        <v>50000000</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+        <v>-100000000</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>97</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>572</v>
+        <v>518</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>565</v>
+        <v>511</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="E81" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="G81" s="4"/>
+        <v>80</v>
+      </c>
       <c r="H81" s="4">
-        <v>-30000000</v>
+        <v>300000000</v>
       </c>
       <c r="I81" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J81" s="4">
-        <v>-30000000</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A82" s="4"/>
-      <c r="B82" s="4"/>
-      <c r="C82" s="4"/>
-      <c r="D82" s="4"/>
-      <c r="E82" s="4"/>
-      <c r="F82" s="4"/>
-      <c r="G82" s="4"/>
-      <c r="H82" s="4"/>
-      <c r="I82" s="4"/>
-      <c r="J82" s="4"/>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+        <v>300000000</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>520</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>511</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>521</v>
+      </c>
+      <c r="E82" s="4">
+        <v>2</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H82" s="4">
+        <v>250000000</v>
+      </c>
+      <c r="I82" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J82" s="4">
+        <v>250000000</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>468</v>
+        <v>522</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>115</v>
+        <v>511</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E83" s="4"/>
+        <v>521</v>
+      </c>
+      <c r="E83" s="4">
+        <v>2</v>
+      </c>
       <c r="F83" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G83" s="4"/>
+        <v>54</v>
+      </c>
       <c r="H83" s="4">
-        <v>10000000</v>
+        <v>-200000000</v>
       </c>
       <c r="I83" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J83" s="4">
-        <v>10000000</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A84" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B84" s="4" t="s">
-        <v>469</v>
-      </c>
-      <c r="C84" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="D84" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E84" s="4"/>
-      <c r="F84" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G84" s="4"/>
-      <c r="H84" s="4">
-        <v>-50000000</v>
-      </c>
-      <c r="I84" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="J84" s="4">
-        <v>-50000000</v>
-      </c>
-    </row>
+        <v>-200000000</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>470</v>
+        <v>564</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>115</v>
+        <v>565</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="E85" s="4"/>
+        <v>512</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F85" s="4" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="G85" s="4"/>
       <c r="H85" s="4">
-        <v>4500000</v>
+        <v>25000000</v>
       </c>
       <c r="I85" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J85" s="4">
-        <v>4500000</v>
+        <v>25000000</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>471</v>
+        <v>566</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>115</v>
+        <v>565</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="E86" s="4"/>
+        <v>514</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F86" s="4" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="G86" s="4"/>
       <c r="H86" s="4">
-        <v>20000000</v>
+        <v>-60000000</v>
       </c>
       <c r="I86" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J86" s="4">
-        <v>20000000</v>
+        <v>-60000000</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>472</v>
+        <v>567</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>115</v>
+        <v>565</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="E87" s="4"/>
+        <v>512</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F87" s="4" t="s">
-        <v>3</v>
+        <v>80</v>
       </c>
       <c r="G87" s="4"/>
       <c r="H87" s="4">
-        <v>-10000000</v>
+        <v>40000000</v>
       </c>
       <c r="I87" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J87" s="4">
-        <v>-10000000</v>
+        <v>40000000</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>473</v>
+        <v>568</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>115</v>
+        <v>565</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="E88" s="4"/>
+        <v>514</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F88" s="4" t="s">
         <v>80</v>
       </c>
       <c r="G88" s="4"/>
       <c r="H88" s="4">
-        <v>90000000</v>
+        <v>30000000</v>
       </c>
       <c r="I88" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J88" s="4">
+        <v>30000000</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>569</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>565</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>514</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G89" s="4"/>
+      <c r="H89" s="4">
+        <v>-15000000</v>
+      </c>
+      <c r="I89" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J89" s="4">
+        <v>-15000000</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>570</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>565</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>519</v>
+      </c>
+      <c r="E90" s="4">
+        <v>1</v>
+      </c>
+      <c r="F90" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G90" s="4"/>
+      <c r="H90" s="4">
+        <v>60000000</v>
+      </c>
+      <c r="I90" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J90" s="4">
+        <v>60000000</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>565</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>521</v>
+      </c>
+      <c r="E91" s="4">
+        <v>2</v>
+      </c>
+      <c r="F91" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G91" s="4"/>
+      <c r="H91" s="4">
+        <v>50000000</v>
+      </c>
+      <c r="I91" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J91" s="4">
+        <v>50000000</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>572</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>565</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>521</v>
+      </c>
+      <c r="E92" s="4">
+        <v>2</v>
+      </c>
+      <c r="F92" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G92" s="4"/>
+      <c r="H92" s="4">
+        <v>-30000000</v>
+      </c>
+      <c r="I92" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J92" s="4">
+        <v>-30000000</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="4"/>
+      <c r="B93" s="4"/>
+      <c r="C93" s="4"/>
+      <c r="D93" s="4"/>
+      <c r="E93" s="4"/>
+      <c r="F93" s="4"/>
+      <c r="G93" s="4"/>
+      <c r="H93" s="4"/>
+      <c r="I93" s="4"/>
+      <c r="J93" s="4"/>
+    </row>
+    <row r="94" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>618</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>625</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E94" s="4">
+        <v>7</v>
+      </c>
+      <c r="F94" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H94" s="4">
+        <v>50000000</v>
+      </c>
+      <c r="I94" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J94" s="4">
+        <v>50000000</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>619</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>625</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>590</v>
+      </c>
+      <c r="E95" s="4">
+        <v>9</v>
+      </c>
+      <c r="F95" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H95" s="4">
+        <v>-400000000</v>
+      </c>
+      <c r="I95" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J95" s="4">
+        <v>-400000000</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>620</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>625</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>590</v>
+      </c>
+      <c r="E96" s="4">
+        <v>9</v>
+      </c>
+      <c r="F96" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H96" s="4">
+        <v>30000000</v>
+      </c>
+      <c r="I96" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J96" s="4">
+        <v>30000000</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>621</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>625</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>602</v>
+      </c>
+      <c r="E97" s="4">
+        <v>11</v>
+      </c>
+      <c r="F97" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H97" s="4">
+        <v>120000000</v>
+      </c>
+      <c r="I97" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J97" s="4">
+        <v>120000000</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>622</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>625</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>602</v>
+      </c>
+      <c r="E98" s="4">
+        <v>11</v>
+      </c>
+      <c r="F98" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H98" s="4">
+        <v>-10000000</v>
+      </c>
+      <c r="I98" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J98" s="4">
+        <v>-10000000</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>623</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>625</v>
+      </c>
+      <c r="D99" s="4" t="s">
+        <v>624</v>
+      </c>
+      <c r="E99" s="4">
+        <v>7</v>
+      </c>
+      <c r="F99" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H99" s="4">
+        <v>100000000</v>
+      </c>
+      <c r="I99" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J99" s="4">
+        <v>100000000</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>468</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E101" s="4"/>
+      <c r="F101" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G101" s="4"/>
+      <c r="H101" s="4">
+        <v>10000000</v>
+      </c>
+      <c r="I101" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J101" s="4">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>469</v>
+      </c>
+      <c r="C102" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D102" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E102" s="4"/>
+      <c r="F102" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G102" s="4"/>
+      <c r="H102" s="4">
+        <v>-50000000</v>
+      </c>
+      <c r="I102" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J102" s="4">
+        <v>-50000000</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="C103" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D103" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E103" s="4"/>
+      <c r="F103" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G103" s="4"/>
+      <c r="H103" s="4">
+        <v>4500000</v>
+      </c>
+      <c r="I103" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J103" s="4">
+        <v>4500000</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="C104" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D104" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E104" s="4"/>
+      <c r="F104" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G104" s="4"/>
+      <c r="H104" s="4">
+        <v>20000000</v>
+      </c>
+      <c r="I104" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J104" s="4">
+        <v>20000000</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>472</v>
+      </c>
+      <c r="C105" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E105" s="4"/>
+      <c r="F105" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G105" s="4"/>
+      <c r="H105" s="4">
+        <v>-10000000</v>
+      </c>
+      <c r="I105" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J105" s="4">
+        <v>-10000000</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="C106" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D106" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E106" s="4"/>
+      <c r="F106" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G106" s="4"/>
+      <c r="H106" s="4">
+        <v>90000000</v>
+      </c>
+      <c r="I106" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J106" s="4">
         <v>90000000</v>
       </c>
     </row>
@@ -8000,7 +9570,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection sqref="A1:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8780,7 +10350,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C5"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fix equity vega. Change risk factors with no tenor
</commit_message>
<xml_diff>
--- a/simm_config.xlsx
+++ b/simm_config.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="632">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="631">
   <si>
     <t>curr</t>
   </si>
@@ -1769,9 +1769,6 @@
   </si>
   <si>
     <t>All S_CNV</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>corr</t>
@@ -2762,8 +2759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C315"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A197" workbookViewId="0">
-      <selection activeCell="C206" sqref="C206"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2792,7 +2789,7 @@
         <v>45</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>580</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3512,7 +3509,7 @@
         <v>232</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -3520,7 +3517,7 @@
         <v>233</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -3528,7 +3525,7 @@
         <v>234</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -3536,7 +3533,7 @@
         <v>235</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -3544,7 +3541,7 @@
         <v>236</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -3552,7 +3549,7 @@
         <v>237</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -3560,7 +3557,7 @@
         <v>238</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -3568,7 +3565,7 @@
         <v>239</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -3576,7 +3573,7 @@
         <v>240</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -3592,7 +3589,7 @@
         <v>242</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -3600,7 +3597,7 @@
         <v>243</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -3608,7 +3605,7 @@
         <v>244</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -3616,7 +3613,7 @@
         <v>245</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -3624,7 +3621,7 @@
         <v>246</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -3632,7 +3629,7 @@
         <v>247</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -3640,7 +3637,7 @@
         <v>248</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -3648,7 +3645,7 @@
         <v>249</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
@@ -3656,7 +3653,7 @@
         <v>250</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
@@ -3664,7 +3661,7 @@
         <v>251</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -3672,7 +3669,7 @@
         <v>252</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
@@ -3680,7 +3677,7 @@
         <v>253</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
@@ -3688,7 +3685,7 @@
         <v>254</v>
       </c>
       <c r="B114" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -4234,7 +4231,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="4" t="s">
         <v>333</v>
       </c>
@@ -4242,7 +4239,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="4" t="s">
         <v>334</v>
       </c>
@@ -4250,7 +4247,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="4" t="s">
         <v>335</v>
       </c>
@@ -4258,7 +4255,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="4" t="s">
         <v>336</v>
       </c>
@@ -4266,7 +4263,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="4" t="s">
         <v>337</v>
       </c>
@@ -4274,7 +4271,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" s="4" t="s">
         <v>338</v>
       </c>
@@ -4282,87 +4279,84 @@
         <v>579</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="4" t="s">
         <v>339</v>
       </c>
       <c r="B199" s="4" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="4" t="s">
         <v>340</v>
       </c>
       <c r="B200" s="4" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" s="4" t="s">
         <v>341</v>
       </c>
       <c r="B201" s="4" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" s="4" t="s">
         <v>342</v>
       </c>
       <c r="B202" s="4" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" s="4" t="s">
         <v>343</v>
       </c>
       <c r="B203" s="4" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" s="4" t="s">
         <v>344</v>
       </c>
       <c r="B204" s="4" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" s="4" t="s">
         <v>345</v>
       </c>
       <c r="B205" s="4" t="s">
-        <v>626</v>
-      </c>
-      <c r="C205" s="5" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="4" t="s">
         <v>346</v>
       </c>
       <c r="B206" s="4" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="4" t="s">
         <v>347</v>
       </c>
       <c r="B207" s="4" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="4" t="s">
         <v>348</v>
       </c>
       <c r="B208" s="4" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
@@ -4370,7 +4364,7 @@
         <v>349</v>
       </c>
       <c r="B209" s="4" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
@@ -4378,7 +4372,7 @@
         <v>350</v>
       </c>
       <c r="B210" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
@@ -5622,7 +5616,7 @@
         <v>19</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -5756,7 +5750,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B2" s="4">
         <v>3100000</v>
@@ -5767,7 +5761,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B3" s="4">
         <v>31000000</v>
@@ -5778,7 +5772,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B4" s="4">
         <v>700000</v>
@@ -5789,7 +5783,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B5" s="4">
         <v>2100000</v>
@@ -5800,7 +5794,7 @@
     </row>
     <row r="6" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B6" s="4">
         <v>690000000</v>
@@ -5822,7 +5816,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B8" s="4">
         <v>1100000000</v>
@@ -5833,7 +5827,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B9" s="4">
         <v>11000000000</v>
@@ -5844,7 +5838,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B10" s="4">
         <v>170000000</v>
@@ -5855,7 +5849,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B11" s="4">
         <v>500000000</v>
@@ -5866,7 +5860,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B12" s="4">
         <v>39000000000</v>
@@ -6006,8 +6000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J106"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="E102" sqref="E102"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7176,13 +7170,13 @@
         <v>76</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>93</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="E42" s="4">
         <v>7</v>
@@ -7202,13 +7196,13 @@
         <v>76</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>93</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="E43" s="4">
         <v>3</v>
@@ -7228,13 +7222,13 @@
         <v>76</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>93</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E44" s="4">
         <v>3</v>
@@ -7254,13 +7248,13 @@
         <v>76</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>93</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="E45" s="4">
         <v>3</v>
@@ -7280,13 +7274,13 @@
         <v>76</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>93</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="E46" s="4">
         <v>9</v>
@@ -7306,13 +7300,13 @@
         <v>76</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>93</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E47" s="4">
         <v>9</v>
@@ -7332,13 +7326,13 @@
         <v>76</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>93</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="E48" s="4">
         <v>10</v>
@@ -7358,13 +7352,13 @@
         <v>76</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>93</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="E49" s="4">
         <v>11</v>
@@ -7384,13 +7378,13 @@
         <v>76</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>93</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="E50" s="4">
         <v>10</v>
@@ -7436,7 +7430,7 @@
         <v>76</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>93</v>
@@ -8484,10 +8478,10 @@
         <v>76</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="D94" s="4" t="s">
         <v>96</v>
@@ -8513,13 +8507,13 @@
         <v>76</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="E95" s="4">
         <v>9</v>
@@ -8542,13 +8536,13 @@
         <v>76</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="E96" s="4">
         <v>9</v>
@@ -8571,13 +8565,13 @@
         <v>76</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="E97" s="4">
         <v>11</v>
@@ -8600,13 +8594,13 @@
         <v>76</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="E98" s="4">
         <v>11</v>
@@ -8629,13 +8623,13 @@
         <v>76</v>
       </c>
       <c r="B99" s="4" t="s">
+        <v>622</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>624</v>
+      </c>
+      <c r="D99" s="4" t="s">
         <v>623</v>
-      </c>
-      <c r="C99" s="4" t="s">
-        <v>625</v>
-      </c>
-      <c r="D99" s="4" t="s">
-        <v>624</v>
       </c>
       <c r="E99" s="4">
         <v>7</v>

</xml_diff>